<commit_message>
Rotational Kinetic Energy and Its Tests
</commit_message>
<xml_diff>
--- a/Hv-calculators/linRotor/cartSphBasis/Hv-calc/MatrixElementTests.xlsx
+++ b/Hv-calculators/linRotor/cartSphBasis/Hv-calc/MatrixElementTests.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="19080" yWindow="1940" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CartesianKineticEnergyOperator" sheetId="1" r:id="rId1"/>
+    <sheet name="RotationalKineticEnergy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>i</t>
   </si>
@@ -67,6 +68,45 @@
   </si>
   <si>
     <t>max difference:</t>
+  </si>
+  <si>
+    <t>mass =</t>
+  </si>
+  <si>
+    <t>g/mol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist = </t>
+  </si>
+  <si>
+    <t>I =</t>
+  </si>
+  <si>
+    <t>(g/mol).nm^2</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Bl(l+1)</t>
+  </si>
+  <si>
+    <t>Code Values</t>
+  </si>
+  <si>
+    <t>B =</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>max:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min: </t>
   </si>
 </sst>
 </file>
@@ -118,8 +158,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,17 +184,21 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1884,4 +1932,2409 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1">
+        <f>2*$B$1*$B$2*$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <f>B3*B3/2/F1</f>
+        <v>2.5207742778390803E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>6.3507785700200006E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>-10</v>
+      </c>
+      <c r="C6">
+        <f>$F$2*A6*(A6+1)</f>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <f>C6-D6</f>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>-9</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C70" si="0">$F$2*A7*(A7+1)</f>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E70" si="1">C7-D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>-9</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>-7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>-7</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>-7</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>-7</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>-6</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>-6</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>-6</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>-6</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>-6</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>-5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>-5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>-5</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>-5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>-5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>-5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>-4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>-4</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>-4</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>-4</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>-4</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>-4</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>-4</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>-3</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>-3</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>-3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D36" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>-3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>-3</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>-3</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>-3</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>-3</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>-2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>1.5124645667034483E-3</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.5124645667034401E-3</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="1"/>
+        <v>8.2399365108898337E-18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>-2</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>-2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>-2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D45" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>-2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>-2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>-2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>-2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D49" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>-2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D50" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>-1</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781607E-4</v>
+      </c>
+      <c r="D51" s="3">
+        <v>5.0415485556781596E-4</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>-1</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>1.5124645667034483E-3</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1.5124645667034401E-3</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="1"/>
+        <v>8.2399365108898337E-18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>-1</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D53" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>-1</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D54" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>-1</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D55" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>-1</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57">
+        <v>-1</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>8</v>
+      </c>
+      <c r="B58">
+        <v>-1</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>-1</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D59" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>-1</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D60" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781607E-4</v>
+      </c>
+      <c r="D62" s="3">
+        <v>5.0415485556781596E-4</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>1.5124645667034483E-3</v>
+      </c>
+      <c r="D63" s="3">
+        <v>1.5124645667034401E-3</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="1"/>
+        <v>8.2399365108898337E-18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D64" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D65" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D66" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D67" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D68" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="1"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D69" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D70" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ref="C71:C126" si="2">$F$2*A71*(A71+1)</f>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D71" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" ref="E71:E126" si="3">C71-D71</f>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="2"/>
+        <v>5.0415485556781607E-4</v>
+      </c>
+      <c r="D72" s="3">
+        <v>5.0415485556781596E-4</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="2"/>
+        <v>1.5124645667034483E-3</v>
+      </c>
+      <c r="D73" s="3">
+        <v>1.5124645667034401E-3</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2399365108898337E-18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D74" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="3"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D75" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E75" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D76" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D77" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D78" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D79" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>9</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D80" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>10</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D81" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="2"/>
+        <v>1.5124645667034483E-3</v>
+      </c>
+      <c r="D82" s="3">
+        <v>1.5124645667034401E-3</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2399365108898337E-18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="2"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D83" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E83" s="3">
+        <f t="shared" si="3"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="2"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D84" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E84" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="2"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D85" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E85" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>6</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E86" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>7</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E87" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>8</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D88" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E88" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>9</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D89" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E89" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>10</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D90" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E90" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="2"/>
+        <v>3.0249291334068966E-3</v>
+      </c>
+      <c r="D91" s="3">
+        <v>3.0249291334068901E-3</v>
+      </c>
+      <c r="E91" s="3">
+        <f t="shared" si="3"/>
+        <v>6.5052130349130266E-18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>3</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="2"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D92" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E92" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="2"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D93" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E93" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D94" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>3</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D95" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E95" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>8</v>
+      </c>
+      <c r="B96">
+        <v>3</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D96" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E96" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D97" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E97" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>10</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D98" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>4</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="2"/>
+        <v>5.0415485556781605E-3</v>
+      </c>
+      <c r="D99" s="3">
+        <v>5.0415485556781596E-3</v>
+      </c>
+      <c r="E99" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="2"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D100" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E100" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>6</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E101" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102">
+        <v>7</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E102" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>4</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E103" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D104" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E104" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105">
+        <v>10</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D105" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E105" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106">
+        <v>5</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="2"/>
+        <v>7.5623228335172411E-3</v>
+      </c>
+      <c r="D106" s="3">
+        <v>7.5623228335172403E-3</v>
+      </c>
+      <c r="E106" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107">
+        <v>6</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D107" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E107" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108">
+        <v>7</v>
+      </c>
+      <c r="B108">
+        <v>5</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E108" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>5</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D109" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E109" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110">
+        <v>9</v>
+      </c>
+      <c r="B110">
+        <v>5</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D110" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E110" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111">
+        <v>10</v>
+      </c>
+      <c r="B111">
+        <v>5</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D111" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E111" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112">
+        <v>6</v>
+      </c>
+      <c r="B112">
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="2"/>
+        <v>1.0587251966924139E-2</v>
+      </c>
+      <c r="D112" s="3">
+        <v>1.05872519669241E-2</v>
+      </c>
+      <c r="E112" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8163916471489756E-17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113">
+        <v>7</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E113" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114">
+        <v>8</v>
+      </c>
+      <c r="B114">
+        <v>6</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D114" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E114" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115">
+        <v>9</v>
+      </c>
+      <c r="B115">
+        <v>6</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D115" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E115" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116">
+        <v>10</v>
+      </c>
+      <c r="B116">
+        <v>6</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D116" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E116" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117">
+        <v>7</v>
+      </c>
+      <c r="B117">
+        <v>7</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="2"/>
+        <v>1.411633595589885E-2</v>
+      </c>
+      <c r="D117" s="3">
+        <v>1.41163359558988E-2</v>
+      </c>
+      <c r="E117" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0306980803327406E-17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118">
+        <v>8</v>
+      </c>
+      <c r="B118">
+        <v>7</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D118" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E118" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119">
+        <v>9</v>
+      </c>
+      <c r="B119">
+        <v>7</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D119" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E119" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120">
+        <v>10</v>
+      </c>
+      <c r="B120">
+        <v>7</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D120" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E120" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121">
+        <v>8</v>
+      </c>
+      <c r="B121">
+        <v>8</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="2"/>
+        <v>1.8149574800441378E-2</v>
+      </c>
+      <c r="D121" s="3">
+        <v>1.8149574800441302E-2</v>
+      </c>
+      <c r="E121" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6327832942979512E-17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122">
+        <v>9</v>
+      </c>
+      <c r="B122">
+        <v>8</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D122" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E122" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123">
+        <v>10</v>
+      </c>
+      <c r="B123">
+        <v>8</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D123" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E123" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>9</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="2"/>
+        <v>2.2686968500551723E-2</v>
+      </c>
+      <c r="D124" s="3">
+        <v>2.2686968500551699E-2</v>
+      </c>
+      <c r="E124" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>10</v>
+      </c>
+      <c r="B125">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D125" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E125" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126">
+        <v>10</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="2"/>
+        <v>2.7728517056229883E-2</v>
+      </c>
+      <c r="D126" s="3">
+        <v>2.77285170562298E-2</v>
+      </c>
+      <c r="E126" s="3">
+        <f t="shared" si="3"/>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="D127" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" s="3">
+        <f>MAX(E6:E126)</f>
+        <v>8.3266726846886741E-17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="D128" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128" s="3">
+        <f>MIN(E6:E126)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>